<commit_message>
Scheduling storing of ratios
</commit_message>
<xml_diff>
--- a/Ratios.xlsx
+++ b/Ratios.xlsx
@@ -3444,7 +3444,7 @@
       </c>
       <c r="AN12" t="inlineStr">
         <is>
-          <t>1,021.64</t>
+          <t>1021.64</t>
         </is>
       </c>
       <c r="AO12" t="inlineStr">
@@ -16134,7 +16134,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>1,045.38</t>
+          <t>1045.38</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -16234,7 +16234,7 @@
       </c>
       <c r="AB62" t="inlineStr">
         <is>
-          <t>1,420.90</t>
+          <t>1420.90</t>
         </is>
       </c>
       <c r="AC62" t="inlineStr">
@@ -16244,12 +16244,12 @@
       </c>
       <c r="AD62" t="inlineStr">
         <is>
-          <t>1,480.21</t>
+          <t>1480.21</t>
         </is>
       </c>
       <c r="AE62" t="inlineStr">
         <is>
-          <t>1,103.87</t>
+          <t>1103.87</t>
         </is>
       </c>
       <c r="AF62" t="inlineStr">
@@ -16491,7 +16491,7 @@
       </c>
       <c r="AB63" t="inlineStr">
         <is>
-          <t>4,439.60</t>
+          <t>4439.60</t>
         </is>
       </c>
       <c r="AC63" t="inlineStr">
@@ -16501,12 +16501,12 @@
       </c>
       <c r="AD63" t="inlineStr">
         <is>
-          <t>4,679.91</t>
+          <t>4679.91</t>
         </is>
       </c>
       <c r="AE63" t="inlineStr">
         <is>
-          <t>3,346.73</t>
+          <t>3346.73</t>
         </is>
       </c>
       <c r="AF63" t="inlineStr">
@@ -16748,7 +16748,7 @@
       </c>
       <c r="AB64" t="inlineStr">
         <is>
-          <t>3,812.16</t>
+          <t>3812.16</t>
         </is>
       </c>
       <c r="AC64" t="inlineStr">
@@ -16758,12 +16758,12 @@
       </c>
       <c r="AD64" t="inlineStr">
         <is>
-          <t>4,031.66</t>
+          <t>4031.66</t>
         </is>
       </c>
       <c r="AE64" t="inlineStr">
         <is>
-          <t>2,954.46</t>
+          <t>2954.46</t>
         </is>
       </c>
       <c r="AF64" t="inlineStr">
@@ -17005,7 +17005,7 @@
       </c>
       <c r="AB65" t="inlineStr">
         <is>
-          <t>5,284.16</t>
+          <t>5284.16</t>
         </is>
       </c>
       <c r="AC65" t="inlineStr">
@@ -17015,12 +17015,12 @@
       </c>
       <c r="AD65" t="inlineStr">
         <is>
-          <t>5,576.70</t>
+          <t>5576.70</t>
         </is>
       </c>
       <c r="AE65" t="inlineStr">
         <is>
-          <t>4,036.08</t>
+          <t>4036.08</t>
         </is>
       </c>
       <c r="AF65" t="inlineStr">
@@ -17579,7 +17579,7 @@
       </c>
       <c r="AN67" t="inlineStr">
         <is>
-          <t>1,967.97</t>
+          <t>1967.97</t>
         </is>
       </c>
       <c r="AO67" t="inlineStr">
@@ -18190,7 +18190,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>1,355.86</t>
+          <t>1355.86</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -18255,12 +18255,12 @@
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>1,359.63</t>
+          <t>1359.63</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>1,359.63</t>
+          <t>1359.63</t>
         </is>
       </c>
       <c r="W70" t="inlineStr">
@@ -18350,7 +18350,7 @@
       </c>
       <c r="AN70" t="inlineStr">
         <is>
-          <t>2,130.65</t>
+          <t>2130.65</t>
         </is>
       </c>
       <c r="AO70" t="inlineStr">
@@ -18405,7 +18405,7 @@
       </c>
       <c r="AY70" t="inlineStr">
         <is>
-          <t>1,359.63</t>
+          <t>1359.63</t>
         </is>
       </c>
     </row>
@@ -18447,7 +18447,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>1,073.20</t>
+          <t>1073.20</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -18607,7 +18607,7 @@
       </c>
       <c r="AN71" t="inlineStr">
         <is>
-          <t>1,792.33</t>
+          <t>1792.33</t>
         </is>
       </c>
       <c r="AO71" t="inlineStr">
@@ -25486,7 +25486,7 @@
       </c>
       <c r="AB98" t="inlineStr">
         <is>
-          <t>1,534.73</t>
+          <t>1534.73</t>
         </is>
       </c>
       <c r="AC98" t="inlineStr">
@@ -25496,12 +25496,12 @@
       </c>
       <c r="AD98" t="inlineStr">
         <is>
-          <t>1,732.37</t>
+          <t>1732.37</t>
         </is>
       </c>
       <c r="AE98" t="inlineStr">
         <is>
-          <t>1,300.44</t>
+          <t>1300.44</t>
         </is>
       </c>
       <c r="AF98" t="inlineStr">
@@ -26257,7 +26257,7 @@
       </c>
       <c r="AB101" t="inlineStr">
         <is>
-          <t>1,060.36</t>
+          <t>1060.36</t>
         </is>
       </c>
       <c r="AC101" t="inlineStr">
@@ -26267,7 +26267,7 @@
       </c>
       <c r="AD101" t="inlineStr">
         <is>
-          <t>1,171.62</t>
+          <t>1171.62</t>
         </is>
       </c>
       <c r="AE101" t="inlineStr">
@@ -27819,7 +27819,7 @@
       </c>
       <c r="AF107" t="inlineStr">
         <is>
-          <t>49,608.00</t>
+          <t>49608.00</t>
         </is>
       </c>
       <c r="AG107" t="inlineStr">
@@ -27829,7 +27829,7 @@
       </c>
       <c r="AH107" t="inlineStr">
         <is>
-          <t>49,608.00</t>
+          <t>49608.00</t>
         </is>
       </c>
       <c r="AI107" t="inlineStr">
@@ -28076,7 +28076,7 @@
       </c>
       <c r="AF108" t="inlineStr">
         <is>
-          <t>8,517.94</t>
+          <t>8517.94</t>
         </is>
       </c>
       <c r="AG108" t="inlineStr">
@@ -28086,7 +28086,7 @@
       </c>
       <c r="AH108" t="inlineStr">
         <is>
-          <t>8,517.94</t>
+          <t>8517.94</t>
         </is>
       </c>
       <c r="AI108" t="inlineStr">
@@ -28141,7 +28141,7 @@
       </c>
       <c r="AS108" t="inlineStr">
         <is>
-          <t>1,261.74</t>
+          <t>1261.74</t>
         </is>
       </c>
       <c r="AT108" t="inlineStr">
@@ -28333,7 +28333,7 @@
       </c>
       <c r="AF109" t="inlineStr">
         <is>
-          <t>15,968.28</t>
+          <t>15968.28</t>
         </is>
       </c>
       <c r="AG109" t="inlineStr">
@@ -28343,7 +28343,7 @@
       </c>
       <c r="AH109" t="inlineStr">
         <is>
-          <t>15,968.28</t>
+          <t>15968.28</t>
         </is>
       </c>
       <c r="AI109" t="inlineStr">
@@ -28590,7 +28590,7 @@
       </c>
       <c r="AF110" t="inlineStr">
         <is>
-          <t>11,377.42</t>
+          <t>11377.42</t>
         </is>
       </c>
       <c r="AG110" t="inlineStr">
@@ -28600,7 +28600,7 @@
       </c>
       <c r="AH110" t="inlineStr">
         <is>
-          <t>11,377.42</t>
+          <t>11377.42</t>
         </is>
       </c>
       <c r="AI110" t="inlineStr">
@@ -28847,7 +28847,7 @@
       </c>
       <c r="AF111" t="inlineStr">
         <is>
-          <t>5,903.87</t>
+          <t>5903.87</t>
         </is>
       </c>
       <c r="AG111" t="inlineStr">
@@ -28857,7 +28857,7 @@
       </c>
       <c r="AH111" t="inlineStr">
         <is>
-          <t>5,903.87</t>
+          <t>5903.87</t>
         </is>
       </c>
       <c r="AI111" t="inlineStr">
@@ -32839,7 +32839,7 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>4,156.12</t>
+          <t>4156.12</t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
@@ -32904,12 +32904,12 @@
       </c>
       <c r="U127" t="inlineStr">
         <is>
-          <t>3,094.29</t>
+          <t>3094.29</t>
         </is>
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>3,094.29</t>
+          <t>3094.29</t>
         </is>
       </c>
       <c r="W127" t="inlineStr">
@@ -33054,7 +33054,7 @@
       </c>
       <c r="AY127" t="inlineStr">
         <is>
-          <t>3,094.29</t>
+          <t>3094.29</t>
         </is>
       </c>
     </row>
@@ -33096,7 +33096,7 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>3,830.22</t>
+          <t>3830.22</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
@@ -33161,12 +33161,12 @@
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>3,270.33</t>
+          <t>3270.33</t>
         </is>
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>3,270.33</t>
+          <t>3270.33</t>
         </is>
       </c>
       <c r="W128" t="inlineStr">
@@ -33311,7 +33311,7 @@
       </c>
       <c r="AY128" t="inlineStr">
         <is>
-          <t>3,270.33</t>
+          <t>3270.33</t>
         </is>
       </c>
     </row>
@@ -33353,7 +33353,7 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>3,419.05</t>
+          <t>3419.05</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
@@ -33418,12 +33418,12 @@
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>2,883.15</t>
+          <t>2883.15</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>2,883.15</t>
+          <t>2883.15</t>
         </is>
       </c>
       <c r="W129" t="inlineStr">
@@ -33568,7 +33568,7 @@
       </c>
       <c r="AY129" t="inlineStr">
         <is>
-          <t>2,883.15</t>
+          <t>2883.15</t>
         </is>
       </c>
     </row>
@@ -33610,7 +33610,7 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>3,089.73</t>
+          <t>3089.73</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
@@ -33675,12 +33675,12 @@
       </c>
       <c r="U130" t="inlineStr">
         <is>
-          <t>3,036.70</t>
+          <t>3036.70</t>
         </is>
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>3,036.70</t>
+          <t>3036.70</t>
         </is>
       </c>
       <c r="W130" t="inlineStr">
@@ -33825,7 +33825,7 @@
       </c>
       <c r="AY130" t="inlineStr">
         <is>
-          <t>3,036.70</t>
+          <t>3036.70</t>
         </is>
       </c>
     </row>
@@ -33867,7 +33867,7 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>3,849.02</t>
+          <t>3849.02</t>
         </is>
       </c>
       <c r="I131" t="inlineStr">
@@ -33932,12 +33932,12 @@
       </c>
       <c r="U131" t="inlineStr">
         <is>
-          <t>2,339.89</t>
+          <t>2339.89</t>
         </is>
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>2,339.89</t>
+          <t>2339.89</t>
         </is>
       </c>
       <c r="W131" t="inlineStr">
@@ -34082,7 +34082,7 @@
       </c>
       <c r="AY131" t="inlineStr">
         <is>
-          <t>2,339.89</t>
+          <t>2339.89</t>
         </is>
       </c>
     </row>
@@ -34124,7 +34124,7 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>1,511.40</t>
+          <t>1511.40</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
@@ -34381,7 +34381,7 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>1,202.01</t>
+          <t>1202.01</t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
@@ -34638,7 +34638,7 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>1,398.25</t>
+          <t>1398.25</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
@@ -34895,7 +34895,7 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>2,618.00</t>
+          <t>2618.00</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
@@ -35152,7 +35152,7 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>3,292.66</t>
+          <t>3292.66</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
@@ -35509,7 +35509,7 @@
       </c>
       <c r="AB137" t="inlineStr">
         <is>
-          <t>1,115.36</t>
+          <t>1115.36</t>
         </is>
       </c>
       <c r="AC137" t="inlineStr">
@@ -35519,7 +35519,7 @@
       </c>
       <c r="AD137" t="inlineStr">
         <is>
-          <t>1,203.02</t>
+          <t>1203.02</t>
         </is>
       </c>
       <c r="AE137" t="inlineStr">
@@ -35776,7 +35776,7 @@
       </c>
       <c r="AD138" t="inlineStr">
         <is>
-          <t>1,080.28</t>
+          <t>1080.28</t>
         </is>
       </c>
       <c r="AE138" t="inlineStr">
@@ -36033,7 +36033,7 @@
       </c>
       <c r="AD139" t="inlineStr">
         <is>
-          <t>1,006.66</t>
+          <t>1006.66</t>
         </is>
       </c>
       <c r="AE139" t="inlineStr">
@@ -38910,7 +38910,7 @@
       </c>
       <c r="AN150" t="inlineStr">
         <is>
-          <t>1,423.46</t>
+          <t>1423.46</t>
         </is>
       </c>
       <c r="AO150" t="inlineStr">
@@ -39167,7 +39167,7 @@
       </c>
       <c r="AN151" t="inlineStr">
         <is>
-          <t>1,357.87</t>
+          <t>1357.87</t>
         </is>
       </c>
       <c r="AO151" t="inlineStr">

</xml_diff>